<commit_message>
Finish Adding Keyboard Shortcuts
The shortcuts currently present will suffice
</commit_message>
<xml_diff>
--- a/Feature Plan.xlsx
+++ b/Feature Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Guest1/IdeaProjects/AudiTranscribe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C139A568-6732-4E47-BA28-F3001ED2D924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8FF248-9261-5C41-9339-2F4DAB101B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8A39A3C6-9572-E947-93B4-701CC8C42CF5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15100" xr2:uid="{8A39A3C6-9572-E947-93B4-701CC8C42CF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -338,16 +338,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -697,7 +697,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA5AA1-A650-E143-A940-8006F2A9B810}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -723,7 +725,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -734,7 +736,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
@@ -743,7 +745,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
@@ -752,7 +754,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
@@ -761,7 +763,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -770,16 +772,16 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
@@ -788,7 +790,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -814,14 +816,14 @@
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -867,7 +869,7 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
@@ -877,7 +879,7 @@
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -886,14 +888,14 @@
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -926,7 +928,7 @@
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="5" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Add a Way to Display Playback Octave
</commit_message>
<xml_diff>
--- a/Feature Plan.xlsx
+++ b/Feature Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Guest1/IdeaProjects/AudiTranscribe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5DC37C-2396-4741-BB53-319018798A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5975989C-08DB-DC4D-8B4B-F8242BCC0925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15100" xr2:uid="{8A39A3C6-9572-E947-93B4-701CC8C42CF5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Version Number</t>
   </si>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA5AA1-A650-E143-A940-8006F2A9B810}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,7 +924,9 @@
       <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">

</xml_diff>

<commit_message>
Add Menu Bar to Spectrogram View
Also added "save as" button to the menu bar
</commit_message>
<xml_diff>
--- a/Feature Plan.xlsx
+++ b/Feature Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Guest1/IdeaProjects/AudiTranscribe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047482A3-5FDE-4249-BC02-D80F8D2BE8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62157D22-3A05-E340-BD76-8423EDE8B256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15100" xr2:uid="{8A39A3C6-9572-E947-93B4-701CC8C42CF5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Version Number</t>
   </si>
@@ -721,7 +721,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A13" sqref="A13:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -866,7 +866,9 @@
       <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
@@ -876,7 +878,9 @@
       <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>

</xml_diff>